<commit_message>
commit new report and new checklist
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111#MGSOFTXX/websapfse/1.0.1/report-checklist.xlsx
+++ b/GATEWAY/A1#111#MGSOFTXX/websapfse/1.0.1/report-checklist.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SALVATORE\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SALVATORE\Desktop\Accreditamento\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11610" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7395" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="1" r:id="rId1"/>
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1074" uniqueCount="465">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1088" uniqueCount="476">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -1721,34 +1721,6 @@
     <t>subject_application_version: V.1.0.1</t>
   </si>
   <si>
-    <t>2025-06-23T11:40:00.5284099Z</t>
-  </si>
-  <si>
-    <t>0HNDI9AJMP05H:00000001</t>
-  </si>
-  <si>
-    <t>"2ecaa2fb-a640-4ee5-8919-c44de849b030"</t>
-  </si>
-  <si>
-    <t>"2025-06-23T19:15:44.7281313Z"</t>
-  </si>
-  <si>
-    <t>0HNDIH92V0VN8:00000004</t>
-  </si>
-  <si>
-    <t>4f37a683-7502-477f-93ee-1262c01d60f3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">        2025-06-24T05:54:45.3769959Z
-</t>
-  </si>
-  <si>
-    <t>a96f2a5dbba491c2d4880c52abcb24b3</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.4.3.2.3e05c26b4c84205b037d4a52adbeb75980db08e9eefbde326335effc5e3ba8c7.80ab0fb359^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>2025-06-24T06:22:13.2915679Z</t>
   </si>
   <si>
@@ -1772,12 +1744,6 @@
     <t>2025-06-24T07:22:03.1303265Z</t>
   </si>
   <si>
-    <t>2025-06-24T07:18:03.3382061Z</t>
-  </si>
-  <si>
-    <t>7227db003c8e4cda6045956505cb8d49</t>
-  </si>
-  <si>
     <t>"title":"Campo token JWT non valido.",
 "detail":"Il campo action_id non è corretto",
 "status":403,"instance":"/jwt-mandatory-field-malformed"</t>
@@ -1791,16 +1757,87 @@
  "status":400,"instance":"/validation/error",</t>
   </si>
   <si>
-    <t>2025-06-25T07:41:24.1233959Z</t>
-  </si>
-  <si>
-    <t>2b5d5073de26ffbb20d350da13e2d8f4</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.4.3.2.3e05c26b4c84205b037d4a52adbeb75980db08e9eefbde326335effc5e3ba8c7.830be2060a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>Errore Gestito Offline prima dell'invio ad Fse, attraverso la validazione su Xsd</t>
+  </si>
+  <si>
+    <t>Errore Gestito Offline prima dell'invio ad Fse</t>
+  </si>
+  <si>
+    <t>2025-06-27T09:23:32.5326369Z2025-06-23T11:40:00.5284099Z</t>
+  </si>
+  <si>
+    <t>d3c8e2f89806d3d482be250acb9ce2fe</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.4.3.2.3e05c26b4c84205b037d4a52adbeb75980db08e9eefbde326335effc5e3ba8c7.5cb1b76972^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Received HTTP response headers after 495.1491ms - 201</t>
+  </si>
+  <si>
+    <t>2025-06-27T11:56:19.802734Z</t>
+  </si>
+  <si>
+    <t>42b39d1d23e5e0ffacced7ccf1524209</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.4.3.2.3e05c26b4c84205b037d4a52adbeb75980db08e9eefbde326335effc5e3ba8c7.ede50334b6^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> HTTP response headers after 512.7817ms - 201</t>
+  </si>
+  <si>
+    <t>2025-06-27T12:32:22.7643981Z</t>
+  </si>
+  <si>
+    <t>110197f55bd529cb85cc641a770db8ae</t>
+  </si>
+  <si>
+    <t>"2025-06-27T12:45:28.910284Z"</t>
+  </si>
+  <si>
+    <t>4ffd81b6f4a7564081c955fc42e1f2be</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.4.3.2.3e05c26b4c84205b037d4a52adbeb75980db08e9eefbde326335effc5e3ba8c7.bfe48c5d7b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2025-06-27T13:15:56.3394214Z</t>
+  </si>
+  <si>
+    <t>9d6de24a9106f319a49c092463b711be</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.4.3.2.3e05c26b4c84205b037d4a52adbeb75980db08e9eefbde326335effc5e3ba8c7.0c9464f96b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2025-06-27T13:32:44.4843036Z</t>
+  </si>
+  <si>
+    <t>2705fc12f62cb6de4923da95c4c35caf</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.4.3.2.3e05c26b4c84205b037d4a52adbeb75980db08e9eefbde326335effc5e3ba8c7.e104b79fb7^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        "title":"Errore semantico.",
+        "detail":"[ERRORE-45| L'elemento 'id' deve contenere gli attributi @root ed @extension valorizzati.],[ERRORE-b169| Sezione Procedura: l'elemento entry/procedure/entryRelationship/supply deve contenere l'elemento id.]",
+        "status":422,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        "type":"/msg/semantic",
+        "title":"Errore semantico.",
+        "detail":"[ERRORE-5| L'elemento ClinicalDocument/confidentialityCode DEVE avere l'attributo @code valorizzato con 'N' o 'R' o 'V', e il @codeSystem='2.16.840.1.113883.5.25'],[ERRORE-45| L'elemento 'id' deve contenere gli attributi @root ed @extension valorizzati.]",
+        "status":422,"instance":"/validation/error",</t>
+  </si>
+  <si>
+    <t>2025-06-27T13:44:57.73072Z</t>
+  </si>
+  <si>
+    <t>916559c7274805c2d0d6fb899f7cb863</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.4.3.2.3e05c26b4c84205b037d4a52adbeb75980db08e9eefbde326335effc5e3ba8c7.9cd514e459^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -2408,6 +2445,9 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2429,9 +2469,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3884,10 +3921,10 @@
   <dimension ref="A1:W752"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B177" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="B148" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="A204" sqref="A204"/>
+      <selection pane="bottomRight" activeCell="A149" sqref="A149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3932,12 +3969,12 @@
       <c r="W1" s="9"/>
     </row>
     <row r="2" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="49" t="s">
+      <c r="A2" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="50"/>
-      <c r="C2" s="51"/>
-      <c r="D2" s="50"/>
+      <c r="B2" s="51"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="51"/>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
       <c r="H2" s="6"/>
@@ -3958,14 +3995,14 @@
       <c r="W2" s="9"/>
     </row>
     <row r="3" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="52" t="s">
+      <c r="A3" s="53" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="53"/>
-      <c r="C3" s="58" t="s">
+      <c r="B3" s="54"/>
+      <c r="C3" s="59" t="s">
         <v>437</v>
       </c>
-      <c r="D3" s="50"/>
+      <c r="D3" s="51"/>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
@@ -3986,12 +4023,12 @@
       <c r="W3" s="9"/>
     </row>
     <row r="4" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="54"/>
-      <c r="B4" s="55"/>
-      <c r="C4" s="58" t="s">
+      <c r="A4" s="55"/>
+      <c r="B4" s="56"/>
+      <c r="C4" s="59" t="s">
         <v>438</v>
       </c>
-      <c r="D4" s="50"/>
+      <c r="D4" s="51"/>
       <c r="E4" s="4"/>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
@@ -4013,12 +4050,12 @@
       <c r="W4" s="9"/>
     </row>
     <row r="5" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="56"/>
-      <c r="B5" s="57"/>
-      <c r="C5" s="58" t="s">
+      <c r="A5" s="57"/>
+      <c r="B5" s="58"/>
+      <c r="C5" s="59" t="s">
         <v>439</v>
       </c>
-      <c r="D5" s="50"/>
+      <c r="D5" s="51"/>
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
@@ -4039,8 +4076,8 @@
       <c r="W5" s="9"/>
     </row>
     <row r="6" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="47"/>
-      <c r="B6" s="48"/>
+      <c r="A6" s="48"/>
+      <c r="B6" s="49"/>
       <c r="C6" s="10"/>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
@@ -9314,16 +9351,16 @@
         <v>293</v>
       </c>
       <c r="F148" s="45">
-        <v>45831</v>
+        <v>45835</v>
       </c>
       <c r="G148" s="46" t="s">
-        <v>440</v>
+        <v>452</v>
       </c>
       <c r="H148" s="46" t="s">
-        <v>441</v>
+        <v>453</v>
       </c>
       <c r="I148" s="46" t="s">
-        <v>442</v>
+        <v>454</v>
       </c>
       <c r="J148" s="38" t="s">
         <v>64</v>
@@ -9337,7 +9374,9 @@
       <c r="Q148" s="38"/>
       <c r="R148" s="38"/>
       <c r="S148" s="38"/>
-      <c r="T148" s="38"/>
+      <c r="T148" s="38" t="s">
+        <v>455</v>
+      </c>
       <c r="U148" s="39"/>
       <c r="V148" s="40"/>
       <c r="W148" s="38" t="s">
@@ -9360,20 +9399,12 @@
       <c r="E149" s="43" t="s">
         <v>292</v>
       </c>
-      <c r="F149" s="37">
-        <v>45831</v>
-      </c>
-      <c r="G149" s="46" t="s">
-        <v>443</v>
-      </c>
-      <c r="H149" s="46" t="s">
-        <v>444</v>
-      </c>
-      <c r="I149" s="46" t="s">
-        <v>445</v>
-      </c>
+      <c r="F149" s="37"/>
+      <c r="G149" s="46"/>
+      <c r="H149" s="46"/>
+      <c r="I149" s="46"/>
       <c r="J149" s="38" t="s">
-        <v>64</v>
+        <v>442</v>
       </c>
       <c r="K149" s="38"/>
       <c r="L149" s="38"/>
@@ -9407,20 +9438,12 @@
       <c r="E150" s="43" t="s">
         <v>279</v>
       </c>
-      <c r="F150" s="37">
-        <v>45832</v>
-      </c>
-      <c r="G150" s="37" t="s">
-        <v>446</v>
-      </c>
-      <c r="H150" s="37" t="s">
-        <v>447</v>
-      </c>
-      <c r="I150" s="42" t="s">
-        <v>448</v>
-      </c>
+      <c r="F150" s="37"/>
+      <c r="G150" s="37"/>
+      <c r="H150" s="37"/>
+      <c r="I150" s="42"/>
       <c r="J150" s="38" t="s">
-        <v>64</v>
+        <v>442</v>
       </c>
       <c r="K150" s="38"/>
       <c r="L150" s="38"/>
@@ -9455,16 +9478,16 @@
         <v>43</v>
       </c>
       <c r="F151" s="37">
-        <v>45832</v>
+        <v>45835</v>
       </c>
       <c r="G151" s="46" t="s">
-        <v>449</v>
+        <v>440</v>
       </c>
       <c r="H151" s="37" t="s">
-        <v>453</v>
+        <v>444</v>
       </c>
       <c r="I151" s="42" t="s">
-        <v>454</v>
+        <v>445</v>
       </c>
       <c r="J151" s="38" t="s">
         <v>64</v>
@@ -9472,13 +9495,13 @@
       <c r="K151" s="38"/>
       <c r="L151" s="38"/>
       <c r="M151" s="38" t="s">
-        <v>450</v>
+        <v>441</v>
       </c>
       <c r="N151" s="38" t="s">
-        <v>451</v>
+        <v>442</v>
       </c>
       <c r="O151" s="38" t="s">
-        <v>452</v>
+        <v>443</v>
       </c>
       <c r="P151" s="38"/>
       <c r="Q151" s="38"/>
@@ -9508,16 +9531,16 @@
         <v>55</v>
       </c>
       <c r="F152" s="37">
-        <v>45832</v>
+        <v>45835</v>
       </c>
       <c r="G152" s="37" t="s">
-        <v>456</v>
+        <v>460</v>
       </c>
       <c r="H152" s="37" t="s">
-        <v>457</v>
+        <v>461</v>
       </c>
       <c r="I152" s="42" t="s">
-        <v>454</v>
+        <v>445</v>
       </c>
       <c r="J152" s="38"/>
       <c r="K152" s="38"/>
@@ -9525,7 +9548,7 @@
       <c r="M152" s="38"/>
       <c r="N152" s="38"/>
       <c r="O152" s="38" t="s">
-        <v>458</v>
+        <v>447</v>
       </c>
       <c r="P152" s="38"/>
       <c r="Q152" s="38"/>
@@ -9558,7 +9581,7 @@
         <v>45832</v>
       </c>
       <c r="G153" s="37" t="s">
-        <v>455</v>
+        <v>446</v>
       </c>
       <c r="H153" s="37"/>
       <c r="I153" s="42"/>
@@ -9572,23 +9595,25 @@
         <v>64</v>
       </c>
       <c r="O153" s="38" t="s">
-        <v>459</v>
+        <v>448</v>
       </c>
       <c r="P153" s="38" t="s">
-        <v>450</v>
+        <v>441</v>
       </c>
       <c r="Q153" s="38" t="s">
-        <v>451</v>
+        <v>442</v>
       </c>
       <c r="R153" s="38" t="s">
-        <v>450</v>
+        <v>441</v>
       </c>
       <c r="S153" s="38" t="s">
-        <v>450</v>
+        <v>441</v>
       </c>
       <c r="T153" s="38"/>
       <c r="U153" s="39"/>
-      <c r="V153" s="40"/>
+      <c r="V153" s="40" t="s">
+        <v>451</v>
+      </c>
       <c r="W153" s="38" t="s">
         <v>44</v>
       </c>
@@ -9610,16 +9635,16 @@
         <v>273</v>
       </c>
       <c r="F154" s="37">
-        <v>45833</v>
+        <v>45835</v>
       </c>
       <c r="G154" s="37" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="H154" s="37" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="I154" s="42" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="J154" s="38" t="s">
         <v>64</v>
@@ -9631,7 +9656,7 @@
         <v>228</v>
       </c>
       <c r="O154" s="38" t="s">
-        <v>460</v>
+        <v>449</v>
       </c>
       <c r="P154" s="38" t="s">
         <v>64</v>
@@ -9699,11 +9724,21 @@
       <c r="E156" s="43" t="s">
         <v>275</v>
       </c>
-      <c r="F156" s="37"/>
-      <c r="G156" s="37"/>
-      <c r="H156" s="37"/>
-      <c r="I156" s="42"/>
-      <c r="J156" s="38"/>
+      <c r="F156" s="37">
+        <v>45835</v>
+      </c>
+      <c r="G156" s="46" t="s">
+        <v>465</v>
+      </c>
+      <c r="H156" s="46" t="s">
+        <v>466</v>
+      </c>
+      <c r="I156" s="42" t="s">
+        <v>467</v>
+      </c>
+      <c r="J156" s="38" t="s">
+        <v>64</v>
+      </c>
       <c r="K156" s="38"/>
       <c r="L156" s="38"/>
       <c r="M156" s="38"/>
@@ -9966,16 +10001,28 @@
       <c r="E163" s="43" t="s">
         <v>271</v>
       </c>
-      <c r="F163" s="37"/>
-      <c r="G163" s="37"/>
-      <c r="H163" s="37"/>
-      <c r="I163" s="42"/>
-      <c r="J163" s="38"/>
+      <c r="F163" s="37">
+        <v>45835</v>
+      </c>
+      <c r="G163" s="46" t="s">
+        <v>468</v>
+      </c>
+      <c r="H163" s="46" t="s">
+        <v>469</v>
+      </c>
+      <c r="I163" s="42" t="s">
+        <v>470</v>
+      </c>
+      <c r="J163" s="38" t="s">
+        <v>64</v>
+      </c>
       <c r="K163" s="38"/>
       <c r="L163" s="38"/>
       <c r="M163" s="38"/>
       <c r="N163" s="38"/>
-      <c r="O163" s="38"/>
+      <c r="O163" s="38" t="s">
+        <v>471</v>
+      </c>
       <c r="P163" s="38"/>
       <c r="Q163" s="38"/>
       <c r="R163" s="38"/>
@@ -10484,11 +10531,21 @@
       <c r="E177" s="43" t="s">
         <v>366</v>
       </c>
-      <c r="F177" s="37"/>
-      <c r="G177" s="37"/>
-      <c r="H177" s="37"/>
-      <c r="I177" s="42"/>
-      <c r="J177" s="38"/>
+      <c r="F177" s="37">
+        <v>45835</v>
+      </c>
+      <c r="G177" s="37" t="s">
+        <v>456</v>
+      </c>
+      <c r="H177" s="37" t="s">
+        <v>457</v>
+      </c>
+      <c r="I177" s="42" t="s">
+        <v>458</v>
+      </c>
+      <c r="J177" s="38" t="s">
+        <v>441</v>
+      </c>
       <c r="K177" s="38"/>
       <c r="L177" s="38"/>
       <c r="M177" s="38"/>
@@ -10498,7 +10555,9 @@
       <c r="Q177" s="38"/>
       <c r="R177" s="38"/>
       <c r="S177" s="38"/>
-      <c r="T177" s="38"/>
+      <c r="T177" s="38" t="s">
+        <v>459</v>
+      </c>
       <c r="U177" s="39"/>
       <c r="V177" s="40"/>
       <c r="W177" s="38" t="s">
@@ -10854,12 +10913,18 @@
       <c r="E187" s="43" t="s">
         <v>410</v>
       </c>
-      <c r="F187" s="59">
-        <v>45833</v>
-      </c>
-      <c r="G187" s="35"/>
-      <c r="H187" s="35"/>
-      <c r="I187" s="35"/>
+      <c r="F187" s="47">
+        <v>45835</v>
+      </c>
+      <c r="G187" s="35" t="s">
+        <v>473</v>
+      </c>
+      <c r="H187" s="35" t="s">
+        <v>474</v>
+      </c>
+      <c r="I187" s="35" t="s">
+        <v>475</v>
+      </c>
       <c r="J187" s="38" t="s">
         <v>64</v>
       </c>
@@ -10869,7 +10934,9 @@
         <v>64</v>
       </c>
       <c r="N187" s="38"/>
-      <c r="O187" s="35"/>
+      <c r="O187" s="38" t="s">
+        <v>472</v>
+      </c>
       <c r="P187" s="38"/>
       <c r="Q187" s="38"/>
       <c r="R187" s="38"/>
@@ -10877,7 +10944,7 @@
       <c r="T187" s="38"/>
       <c r="U187" s="35"/>
       <c r="V187" s="35" t="s">
-        <v>464</v>
+        <v>450</v>
       </c>
       <c r="W187" s="35" t="s">
         <v>44</v>
@@ -17375,27 +17442,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A92AB09DCDF6014AA0D6826BF29E2C8E" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d4db60622090a1f8a8d506ac1d64a349">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1e76d14e-d0ce-457c-8343-9b55836d9ead" xmlns:ns3="a56712a3-8dfd-4688-917a-22f0cf513b89" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0a3a9ed8bb952a3d76dd1e2fa3d624b9" ns2:_="" ns3:_="">
     <xsd:import namespace="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
@@ -17653,10 +17699,42 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ACB08642-5694-4F88-BF6F-98521E3A5E0B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
+    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -17679,20 +17757,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ACB08642-5694-4F88-BF6F-98521E3A5E0B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
-    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>